<commit_message>
Se cambió la estructura de la tabla folio. Revisar la estructura de tablas del archivo de Excel
</commit_message>
<xml_diff>
--- a/1 Sistema/Base de Datos/Tablas DB.xlsx
+++ b/1 Sistema/Base de Datos/Tablas DB.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELFINO\Google Drive\Proyecto Mixiote\1 Sistema\Base de Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6AE704DF-9946-4271-8858-77C13DEABD52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9CE040CA-A930-4B98-AFC6-4B47C8B0B484}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{240CC93E-1273-4AD3-BBCC-31D6B1937CF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -79,8 +79,79 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Antes era idMesero.
-Se realizó el cambio porque a veces los volanteros llegan a realizar la función de los meseros.</t>
+Se decidió eliminar la llave foránea para porder almacenar más de una mesa. Sucede lo mismo con el campo "mesa"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{9621838A-C4E4-4F8C-AC6C-6E59C3C2C74D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DELFINO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Se cambió el tipo de dato a SmallDateTime debido a problemas de conversión de tipos en C#</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{30399000-F478-422A-A2AC-FC0F7ADD6375}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DELFINO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Se cambió el tipo de dato a SmallDateTime debido a problemas de conversión de tipos en C#</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{9ED00BBB-9DF9-427B-97B1-906744385C48}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DELFINO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Se cambió el tipo de dato a SmallDateTime debido a problemas de conversión de tipos en C#</t>
         </r>
       </text>
     </comment>
@@ -587,7 +658,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">time </t>
+      <t xml:space="preserve">decimal (6,2) </t>
     </r>
     <r>
       <rPr>
@@ -601,7 +672,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">decimal (6,2) </t>
+      <t xml:space="preserve">varchar (30) </t>
     </r>
     <r>
       <rPr>
@@ -615,7 +686,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">varchar (30) </t>
+      <t xml:space="preserve">varchar (10) </t>
     </r>
     <r>
       <rPr>
@@ -629,7 +700,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">varchar (10) </t>
+      <t xml:space="preserve">varchar (12) </t>
     </r>
     <r>
       <rPr>
@@ -643,7 +714,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">varchar (12) </t>
+      <t xml:space="preserve">varchar (60) </t>
     </r>
     <r>
       <rPr>
@@ -657,7 +728,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">varchar (60) </t>
+      <t xml:space="preserve">double (6,2) </t>
     </r>
     <r>
       <rPr>
@@ -671,7 +742,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">double (6,2) </t>
+      <t xml:space="preserve">varchar (70) </t>
     </r>
     <r>
       <rPr>
@@ -685,7 +756,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">varchar (70) </t>
+      <t xml:space="preserve">dateTime </t>
     </r>
     <r>
       <rPr>
@@ -699,7 +770,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">dateTime </t>
+      <t xml:space="preserve">varchar (50) </t>
     </r>
     <r>
       <rPr>
@@ -712,8 +783,11 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">varchar (50) </t>
+    <t xml:space="preserve">varchar (30) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (100) </t>
     </r>
     <r>
       <rPr>
@@ -722,15 +796,21 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Not Null</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">varchar (30) </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">varchar (100) </t>
+      <t xml:space="preserve">Not Null </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="8" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Default 'NA'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (70) </t>
     </r>
     <r>
       <rPr>
@@ -748,12 +828,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Default 'NA'</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">varchar (70) </t>
+      <t xml:space="preserve">Default 'NA' </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (12) </t>
     </r>
     <r>
       <rPr>
@@ -771,12 +851,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Default 'NA' </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">varchar (12) </t>
+      <t>Default 'NA'</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (30) </t>
     </r>
     <r>
       <rPr>
@@ -799,7 +879,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">varchar (30) </t>
+      <t xml:space="preserve">varchar (70) </t>
     </r>
     <r>
       <rPr>
@@ -821,8 +901,17 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">varchar (70) </t>
+    <t>Cortesia</t>
+  </si>
+  <si>
+    <t>int identity(1,1)</t>
+  </si>
+  <si>
+    <t>descuento</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">varchar (7) </t>
     </r>
     <r>
       <rPr>
@@ -831,30 +920,12 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Not Null </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="8" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Default 'NA'</t>
-    </r>
-  </si>
-  <si>
-    <t>Cortesia</t>
-  </si>
-  <si>
-    <t>int identity(1,1)</t>
-  </si>
-  <si>
-    <t>descuento</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">varchar (7) </t>
+      <t>Not Null</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SmallDateTime </t>
     </r>
     <r>
       <rPr>
@@ -2968,14 +3039,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A028D55A-9A93-42A3-A675-5F246989E934}">
   <dimension ref="C2:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
     <col min="9" max="10" width="16.5703125" customWidth="1"/>
@@ -3065,7 +3136,7 @@
         <v>17</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>38</v>
@@ -3081,7 +3152,7 @@
       </c>
     </row>
     <row r="5" spans="3:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="20" t="s">
@@ -3097,13 +3168,13 @@
         <v>18</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>29</v>
@@ -3129,13 +3200,13 @@
         <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>18</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="3:16" ht="30" x14ac:dyDescent="0.25">
@@ -3155,13 +3226,13 @@
         <v>64</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="3:16" ht="30" x14ac:dyDescent="0.25">
@@ -3169,19 +3240,19 @@
         <v>10</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="3:16" ht="31.5" x14ac:dyDescent="0.25">
@@ -3189,7 +3260,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>62</v>
@@ -3215,7 +3286,7 @@
         <v>4</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>6</v>
@@ -3267,7 +3338,7 @@
         <v>22</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>65</v>
@@ -3281,7 +3352,7 @@
         <v>61</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L13" s="2" t="s">
         <v>66</v>
@@ -3371,19 +3442,19 @@
         <v>42</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>45</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="3:16" ht="45" x14ac:dyDescent="0.25">
@@ -3403,19 +3474,19 @@
         <v>43</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="3:16" ht="30" x14ac:dyDescent="0.25">
@@ -3429,13 +3500,13 @@
         <v>7</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>46</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>37</v>
@@ -3455,13 +3526,13 @@
         <v>47</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>48</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
@@ -3486,7 +3557,7 @@
         <v>31</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>31</v>
@@ -3503,13 +3574,13 @@
         <v>56</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I28" s="12" t="s">
         <v>6</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="3:16" ht="30" x14ac:dyDescent="0.25">
@@ -3517,13 +3588,13 @@
         <v>52</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I29" s="16" t="s">
         <v>1</v>
@@ -3537,19 +3608,19 @@
         <v>53</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>58</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="3:16" ht="30" x14ac:dyDescent="0.25">
@@ -3557,7 +3628,7 @@
         <v>20</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.25">
@@ -3573,7 +3644,7 @@
         <v>15</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="3:4" ht="30" x14ac:dyDescent="0.25">
@@ -3581,7 +3652,7 @@
         <v>21</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">

</xml_diff>